<commit_message>
Add updated Excel file of Indicators Series ID, add update tile_map.py to include correct directory path as well as custom hover options
</commit_message>
<xml_diff>
--- a/Indicators Series ID List.xlsx
+++ b/Indicators Series ID List.xlsx
@@ -7,19 +7,51 @@
     <sheet state="visible" name="MD IPUMS NHGIS" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="COUNTY FRED" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="COUNTY BLS" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="MD SOCRATA" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="6R8bCbvsubHGIDJdL+kMdsloxLiPwHIuDtnFK3LoPQ0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="LtQCjL/RKzHEGKYYnaBBEX0nPbqUTXgEi74MEnU3Rrw="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A2">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABxAg8WmY
+Lily Gates-Van Hout    (2025-12-04 15:52:33)
+Desired data output: https://docs.google.com/spreadsheets/d/1eoeoVheT_wAcfjPlPO2eU1FFSgRHtKc3/edit?gid=469139113#gid=469139113</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A1">
+      <text>
+        <t xml:space="preserve">======
+ID#AAABxAg8WmU
+Lily Gates-Van Hout    (2025-12-04 15:51:52)
+To be added: https://dev.socrata.com/foundry/opendata.maryland.gov/w3bc-8mnv</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgvKxwnHoSAl0XaUNRqTD/+xlJ00Q=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="841">
   <si>
     <t>DATA TYPE</t>
   </si>
@@ -2536,13 +2568,19 @@
   </si>
   <si>
     <t>LAUCN240470000000005</t>
+  </si>
+  <si>
+    <t>https://dev.socrata.com/foundry/opendata.maryland.gov/w3bc-8mnv</t>
+  </si>
+  <si>
+    <t>Foreclosure Notice for All Counties (MONTHLY).xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -2706,6 +2744,15 @@
       <color rgb="FF548135"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2795,7 +2842,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2937,6 +2984,12 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3008,6 +3061,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -6490,7 +6547,10 @@
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="C2" sqref="C2" pane="topRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
@@ -9601,4 +9661,37 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="56.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="55" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="56" t="s">
+        <v>840</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="A1"/>
+    <hyperlink r:id="rId3" location="gid=469139113" ref="A2"/>
+  </hyperlinks>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>